<commit_message>
made knn and multioutpu in scratch
</commit_message>
<xml_diff>
--- a/Django/eightsemproject/attendance_records.xlsx
+++ b/Django/eightsemproject/attendance_records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,9 +461,54 @@
           <t>sumit bam</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8</t>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-08-06</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sauju basnet</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-08-07</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sumit bam</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-08-07</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sauju basnet</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>7</t>
         </is>
       </c>
     </row>

</xml_diff>